<commit_message>
Minimal tabular data for references
</commit_message>
<xml_diff>
--- a/tabular/core/hiv-reference-data.xlsx
+++ b/tabular/core/hiv-reference-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/Ortervirales/HIV-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2335B1B-48A3-694E-96C5-BD1AF69F0513}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6B59B0-06E5-6947-8F26-D73466C9E41D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15340" yWindow="9280" windowWidth="27240" windowHeight="16440" xr2:uid="{42735871-A8C7-D842-BA39-4089F1652FC4}"/>
   </bookViews>
@@ -1018,11 +1018,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685A96F8-87E5-2E44-B73D-ACDE15C469C7}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="10" max="10" width="24.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Restricted to primate lentiviruses only
</commit_message>
<xml_diff>
--- a/tabular/core/hiv-reference-data.xlsx
+++ b/tabular/core/hiv-reference-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/Ortervirales/HIV-GLUE/tabular/core/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/general/HIV-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6B59B0-06E5-6947-8F26-D73466C9E41D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952F9B2A-80F5-2240-865C-DD44B1F9FE81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15340" yWindow="9280" windowWidth="27240" windowHeight="16440" xr2:uid="{42735871-A8C7-D842-BA39-4089F1652FC4}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="156">
   <si>
     <t>Accession</t>
   </si>
@@ -480,90 +480,6 @@
     <t>Piliocolobus badius</t>
   </si>
   <si>
-    <t>M32690</t>
-  </si>
-  <si>
-    <t>NPLV</t>
-  </si>
-  <si>
-    <t>BIV</t>
-  </si>
-  <si>
-    <t>cattle</t>
-  </si>
-  <si>
-    <t>Bos taurus</t>
-  </si>
-  <si>
-    <t>U21603</t>
-  </si>
-  <si>
-    <t>JDV</t>
-  </si>
-  <si>
-    <t>Jembrana</t>
-  </si>
-  <si>
-    <t>Bali cattle</t>
-  </si>
-  <si>
-    <t>Bos javanicus</t>
-  </si>
-  <si>
-    <t>M16575</t>
-  </si>
-  <si>
-    <t>EIAV</t>
-  </si>
-  <si>
-    <t>horse</t>
-  </si>
-  <si>
-    <t>Equus ferus</t>
-  </si>
-  <si>
-    <t>M25381</t>
-  </si>
-  <si>
-    <t>FIV</t>
-  </si>
-  <si>
-    <t>FIV_P</t>
-  </si>
-  <si>
-    <t>cat</t>
-  </si>
-  <si>
-    <t>Felis catus</t>
-  </si>
-  <si>
-    <t>M60610</t>
-  </si>
-  <si>
-    <t>SRLV</t>
-  </si>
-  <si>
-    <t>SRLV-A</t>
-  </si>
-  <si>
-    <t>sheep</t>
-  </si>
-  <si>
-    <t>Ovis aries</t>
-  </si>
-  <si>
-    <t>M33677</t>
-  </si>
-  <si>
-    <t>SRLV-B</t>
-  </si>
-  <si>
-    <t>goat</t>
-  </si>
-  <si>
-    <t>Capra aegagrus</t>
-  </si>
-  <si>
     <t>KP861923</t>
   </si>
   <si>
@@ -580,6 +496,9 @@
   </si>
   <si>
     <t>Pan troglodytes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -610,7 +529,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -632,12 +551,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD9D9D9"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -678,7 +591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -695,10 +608,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1016,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685A96F8-87E5-2E44-B73D-ACDE15C469C7}">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection sqref="A1:K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1352,31 +1261,31 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>177</v>
+        <v>149</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>178</v>
+        <v>150</v>
       </c>
       <c r="E11" t="s">
-        <v>179</v>
+        <v>151</v>
       </c>
       <c r="F11" t="s">
-        <v>180</v>
-      </c>
-      <c r="G11" s="10">
+        <v>152</v>
+      </c>
+      <c r="G11" s="8">
         <v>2005</v>
       </c>
       <c r="H11" t="s">
         <v>32</v>
       </c>
       <c r="I11" t="s">
-        <v>181</v>
+        <v>153</v>
       </c>
       <c r="J11" t="s">
-        <v>182</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -1937,148 +1846,9 @@
         <v>148</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>149</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="G31" s="9"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="J31" s="8" t="s">
-        <v>153</v>
-      </c>
-    </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>154</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="7" t="s">
         <v>155</v>
-      </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="G32" s="9"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="J32" s="8" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>159</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="G33" s="9"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="J33" s="8" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>163</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="G34" s="9"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="J34" s="8" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>168</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="G35" s="9"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="J35" s="8" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>173</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="G36" s="9"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="J36" s="8" t="s">
-        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes associated with more narrow scope
</commit_message>
<xml_diff>
--- a/tabular/core/hiv-reference-data.xlsx
+++ b/tabular/core/hiv-reference-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/general/HIV-GLUE/tabular/core/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samanthacampbell/glue_repos/HIV-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E890258-25FA-C64D-936F-6BB9421E2CA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFF9A86-75FE-4849-B101-597D6D5CE250}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15340" yWindow="9280" windowWidth="27240" windowHeight="16440" xr2:uid="{42735871-A8C7-D842-BA39-4089F1652FC4}"/>
+    <workbookView xWindow="5100" yWindow="3060" windowWidth="27240" windowHeight="16440" xr2:uid="{42735871-A8C7-D842-BA39-4089F1652FC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
   <si>
     <t>Accession</t>
   </si>
@@ -93,33 +93,12 @@
     <t>Homo sapiens</t>
   </si>
   <si>
-    <t>NC_001802</t>
-  </si>
-  <si>
-    <t>AF484509</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
-    <t>98UG57136</t>
-  </si>
-  <si>
-    <t>Uganda</t>
-  </si>
-  <si>
-    <t>U46016</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
-    <t>ETH2220</t>
-  </si>
-  <si>
-    <t>Ethiopia</t>
-  </si>
-  <si>
     <t>DQ017382</t>
   </si>
   <si>
@@ -184,6 +163,24 @@
   </si>
   <si>
     <t>Pan troglodytes</t>
+  </si>
+  <si>
+    <t>U52953</t>
+  </si>
+  <si>
+    <t>AF004885</t>
+  </si>
+  <si>
+    <t>Q23-CxC</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>92BR025</t>
   </si>
 </sst>
 </file>
@@ -610,14 +607,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685A96F8-87E5-2E44-B73D-ACDE15C469C7}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A10"/>
+      <selection activeCell="K9" sqref="A1:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
     <col min="10" max="10" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -691,7 +689,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>12</v>
@@ -703,16 +701,16 @@
         <v>14</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="G3" s="6">
-        <v>1983</v>
+        <v>1994</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>18</v>
@@ -721,12 +719,12 @@
         <v>19</v>
       </c>
       <c r="K3" s="6">
-        <v>9362478</v>
+        <v>12487816</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>12</v>
@@ -738,16 +736,16 @@
         <v>14</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="G4" s="6">
-        <v>1998</v>
+        <v>1992</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>18</v>
@@ -756,12 +754,12 @@
         <v>19</v>
       </c>
       <c r="K4" s="6">
-        <v>12487816</v>
+        <v>8891112</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>12</v>
@@ -770,33 +768,28 @@
         <v>13</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="G5" s="6">
-        <v>1986</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>28</v>
+        <v>2004</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>18</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="K5" s="6">
-        <v>8891112</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>12</v>
@@ -805,17 +798,17 @@
         <v>13</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G6" s="6">
-        <v>2004</v>
+        <v>1991</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>18</v>
@@ -826,26 +819,26 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G7" s="6">
-        <v>1991</v>
+        <v>2006</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>18</v>
@@ -856,91 +849,61 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="6">
-        <v>2006</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>19</v>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="8">
+        <v>2005</v>
+      </c>
+      <c r="H8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" s="8">
-        <v>2005</v>
-      </c>
-      <c r="H9" t="s">
-        <v>32</v>
-      </c>
-      <c r="I9" t="s">
-        <v>49</v>
-      </c>
-      <c r="J9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G10" s="6">
+      <c r="C9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="6">
         <v>2004</v>
       </c>
-      <c r="H10" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>44</v>
+      <c r="H9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Valid build with minimal HIV-1 and SIVcpz/SIVgor references
</commit_message>
<xml_diff>
--- a/tabular/core/hiv-reference-data.xlsx
+++ b/tabular/core/hiv-reference-data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samanthacampbell/glue_repos/HIV-GLUE/tabular/core/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/general/HIV-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFF9A86-75FE-4849-B101-597D6D5CE250}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A519112-BFD3-1D42-A37F-0D65C2C52AB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="3060" windowWidth="27240" windowHeight="16440" xr2:uid="{42735871-A8C7-D842-BA39-4089F1652FC4}"/>
+    <workbookView xWindow="27560" yWindow="460" windowWidth="20380" windowHeight="18480" xr2:uid="{42735871-A8C7-D842-BA39-4089F1652FC4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="main refs" sheetId="1" r:id="rId1"/>
+    <sheet name="excluded" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="62">
   <si>
     <t>Accession</t>
   </si>
@@ -153,18 +154,9 @@
     <t>SIVcpz</t>
   </si>
   <si>
-    <t>cpz</t>
-  </si>
-  <si>
     <t>LB715</t>
   </si>
   <si>
-    <t>chimpazee</t>
-  </si>
-  <si>
-    <t>Pan troglodytes</t>
-  </si>
-  <si>
     <t>U52953</t>
   </si>
   <si>
@@ -181,6 +173,51 @@
   </si>
   <si>
     <t>92BR025</t>
+  </si>
+  <si>
+    <t>X52154</t>
+  </si>
+  <si>
+    <t>AF103818</t>
+  </si>
+  <si>
+    <t>JN091691</t>
+  </si>
+  <si>
+    <t>ptt</t>
+  </si>
+  <si>
+    <t>pts</t>
+  </si>
+  <si>
+    <t>Pan troglodytes troglodytes</t>
+  </si>
+  <si>
+    <t>Tanzania</t>
+  </si>
+  <si>
+    <t>Pan troglodytes schweinfurthii</t>
+  </si>
+  <si>
+    <t>TAN5</t>
+  </si>
+  <si>
+    <t>chimpanzee</t>
+  </si>
+  <si>
+    <t>US-Marilyn</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>NK</t>
+  </si>
+  <si>
+    <t>AY618998</t>
+  </si>
+  <si>
+    <t>pCMO2.3</t>
   </si>
 </sst>
 </file>
@@ -273,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -287,10 +324,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -607,15 +640,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685A96F8-87E5-2E44-B73D-ACDE15C469C7}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="A1:K9"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="9" max="9" width="16.83203125" customWidth="1"/>
     <col min="10" max="10" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -655,7 +689,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -670,26 +704,28 @@
       <c r="E2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G2" s="6">
         <v>1983</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="6"/>
+      <c r="K2" s="6" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>45</v>
+      <c r="A3" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>12</v>
@@ -703,19 +739,19 @@
       <c r="E3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>46</v>
+      <c r="F3" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="G3" s="6">
         <v>1994</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I3" s="5" t="s">
+      <c r="H3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="6" t="s">
         <v>19</v>
       </c>
       <c r="K3" s="6">
@@ -723,8 +759,8 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>44</v>
+      <c r="A4" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>12</v>
@@ -738,19 +774,19 @@
       <c r="E4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>49</v>
+      <c r="F4" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="G4" s="6">
         <v>1992</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" s="5" t="s">
+      <c r="H4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="6" t="s">
         <v>19</v>
       </c>
       <c r="K4" s="6">
@@ -758,7 +794,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -780,16 +816,19 @@
       <c r="H5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="6" t="s">
         <v>19</v>
+      </c>
+      <c r="K5" s="6">
+        <v>16438650</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>12</v>
@@ -802,108 +841,336 @@
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="6">
-        <v>1991</v>
+        <v>61</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="K6" s="6" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>29</v>
+      <c r="A7" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G7" s="6">
-        <v>2006</v>
+        <v>1991</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="K7" s="6">
+        <v>8107219</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="6">
+        <v>2006</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="6">
+        <v>21084486</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E8" t="s">
+      <c r="D9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="8">
+      <c r="G9" s="6">
         <v>2005</v>
-      </c>
-      <c r="H8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" t="s">
-        <v>42</v>
-      </c>
-      <c r="J8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="6">
-        <v>2004</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K9" s="6">
+        <v>25900654</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="6">
+        <v>2004</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J10" s="6" t="s">
         <v>37</v>
+      </c>
+      <c r="K10" s="6">
+        <v>19073717</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11" s="6">
+        <v>2188136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K12" s="6">
+        <v>9989410</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="6">
+        <v>2006</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="K13" s="6">
+        <v>21775446</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C898F709-88FD-7D4F-BCC8-2857C1587A7E}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="A2:K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="6">
+        <v>1991</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="6">
+        <v>8107219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated side data, removed lockfile
</commit_message>
<xml_diff>
--- a/tabular/core/hiv-reference-data.xlsx
+++ b/tabular/core/hiv-reference-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/general/HIV-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A519112-BFD3-1D42-A37F-0D65C2C52AB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6FDB761-DE80-154B-8BFE-CFFFD4C4AC49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27560" yWindow="460" windowWidth="20380" windowHeight="18480" xr2:uid="{42735871-A8C7-D842-BA39-4089F1652FC4}"/>
   </bookViews>
@@ -643,7 +643,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="K13" sqref="A1:K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Removed redundant taxonomic field 'subgroup'
</commit_message>
<xml_diff>
--- a/tabular/core/hiv-reference-data.xlsx
+++ b/tabular/core/hiv-reference-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/general/HIV-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6FDB761-DE80-154B-8BFE-CFFFD4C4AC49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF858BA-69F0-744D-9FAD-663F6CE97BE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27560" yWindow="460" windowWidth="20380" windowHeight="18480" xr2:uid="{42735871-A8C7-D842-BA39-4089F1652FC4}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="62">
   <si>
     <t>Accession</t>
   </si>
@@ -187,9 +187,6 @@
     <t>ptt</t>
   </si>
   <si>
-    <t>pts</t>
-  </si>
-  <si>
     <t>Pan troglodytes troglodytes</t>
   </si>
   <si>
@@ -218,6 +215,9 @@
   </si>
   <si>
     <t>pCMO2.3</t>
+  </si>
+  <si>
+    <t>Western</t>
   </si>
 </sst>
 </file>
@@ -640,453 +640,414 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685A96F8-87E5-2E44-B73D-ACDE15C469C7}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="A1:K13"/>
+      <selection activeCell="J13" sqref="A1:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="9" max="9" width="16.83203125" customWidth="1"/>
-    <col min="10" max="10" width="24.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="H1" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="6">
+      <c r="F2" s="6">
         <v>1983</v>
       </c>
+      <c r="G2" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="H2" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="6">
+      <c r="F3" s="6">
         <v>1994</v>
       </c>
+      <c r="G3" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="H3" s="6" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="6">
+      <c r="J3" s="6">
         <v>12487816</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="C4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="6">
+      <c r="F4" s="6">
         <v>1992</v>
       </c>
+      <c r="G4" s="6" t="s">
+        <v>45</v>
+      </c>
       <c r="H4" s="6" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="6">
+      <c r="J4" s="6">
         <v>8891112</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6" t="s">
+      <c r="D5" s="6"/>
+      <c r="E5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="6">
+      <c r="F5" s="6">
         <v>2004</v>
       </c>
+      <c r="G5" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="H5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="6">
+        <v>16438650</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="6">
-        <v>16438650</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="J6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="C7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6" t="s">
+      <c r="D7" s="6"/>
+      <c r="E7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="6">
+      <c r="F7" s="6">
         <v>1991</v>
       </c>
+      <c r="G7" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="H7" s="6" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K7" s="6">
+      <c r="J7" s="6">
         <v>8107219</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>12</v>
+      <c r="B8" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6" t="s">
+      <c r="D8" s="6"/>
+      <c r="E8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="6">
+      <c r="F8" s="6">
         <v>2006</v>
       </c>
+      <c r="G8" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="H8" s="6" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="6">
+      <c r="J8" s="6">
         <v>21084486</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>12</v>
+      <c r="B9" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6" t="s">
+      <c r="D9" s="6"/>
+      <c r="E9" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="6">
+      <c r="F9" s="6">
         <v>2005</v>
       </c>
+      <c r="G9" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="H9" s="6" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="K9" s="6">
+        <v>51</v>
+      </c>
+      <c r="J9" s="6">
         <v>25900654</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>12</v>
+      <c r="B10" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6" t="s">
+      <c r="D10" s="6"/>
+      <c r="E10" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="6">
+      <c r="F10" s="6">
         <v>2004</v>
       </c>
+      <c r="G10" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="H10" s="6" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J10" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="K10" s="6">
+      <c r="J10" s="6">
         <v>19073717</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>12</v>
+      <c r="B11" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6" t="s">
+        <v>58</v>
+      </c>
       <c r="F11" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="K11" s="6">
+        <v>51</v>
+      </c>
+      <c r="J11" s="6">
         <v>2188136</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>12</v>
+      <c r="B12" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="F12" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="K12" s="6">
+        <v>51</v>
+      </c>
+      <c r="J12" s="6">
         <v>9989410</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>12</v>
+      <c r="B13" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="6">
+        <v>2006</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="6">
-        <v>2006</v>
-      </c>
-      <c r="H13" s="6" t="s">
+      <c r="I13" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="I13" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="K13" s="6">
+      <c r="J13" s="6">
         <v>21775446</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More complete reference data
</commit_message>
<xml_diff>
--- a/tabular/core/hiv-reference-data.xlsx
+++ b/tabular/core/hiv-reference-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/general/HIV-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2256605B-CE77-B44A-8EEE-C6AB5757899C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FFC595-986F-F848-A21B-5C4D180B8142}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25740" yWindow="4960" windowWidth="20380" windowHeight="18480" xr2:uid="{42735871-A8C7-D842-BA39-4089F1652FC4}"/>
+    <workbookView xWindow="29900" yWindow="4100" windowWidth="20380" windowHeight="18480" xr2:uid="{42735871-A8C7-D842-BA39-4089F1652FC4}"/>
   </bookViews>
   <sheets>
     <sheet name="main refs" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="101">
   <si>
     <t>Accession</t>
   </si>
@@ -302,6 +302,39 @@
   </si>
   <si>
     <t>China</t>
+  </si>
+  <si>
+    <t>pZAC</t>
+  </si>
+  <si>
+    <t>DEMA112UA014</t>
+  </si>
+  <si>
+    <t>LA21LeAn</t>
+  </si>
+  <si>
+    <t>URTR35</t>
+  </si>
+  <si>
+    <t>Fj061</t>
+  </si>
+  <si>
+    <t>pXJDC6291-2-6</t>
+  </si>
+  <si>
+    <t>Democratic Republic of the Congo</t>
+  </si>
+  <si>
+    <t>LA19KoSa</t>
+  </si>
+  <si>
+    <t>LA49RBF189</t>
+  </si>
+  <si>
+    <t>RBF168</t>
+  </si>
+  <si>
+    <t>YBF30</t>
   </si>
 </sst>
 </file>
@@ -751,7 +784,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="A1:J17"/>
+      <selection activeCell="J16" sqref="A1:J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -840,8 +873,13 @@
       <c r="D3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="G3" t="s">
+      <c r="E3" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1981</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>86</v>
       </c>
       <c r="H3" s="5" t="s">
@@ -849,6 +887,9 @@
       </c>
       <c r="I3" s="5" t="s">
         <v>16</v>
+      </c>
+      <c r="J3" s="5">
+        <v>23170185</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -864,8 +905,13 @@
       <c r="D4" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="G4" t="s">
+      <c r="E4" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4" s="5">
+        <v>2012</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>87</v>
       </c>
       <c r="H4" s="5" t="s">
@@ -873,6 +919,9 @@
       </c>
       <c r="I4" s="5" t="s">
         <v>16</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -888,15 +937,24 @@
       <c r="D5" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="E5" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F5" s="5">
+        <v>2003</v>
+      </c>
+      <c r="G5" s="5"/>
       <c r="H5" s="5" t="s">
         <v>68</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+      <c r="J5" s="5">
+        <v>26699702</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>73</v>
       </c>
@@ -909,8 +967,13 @@
       <c r="D6" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="G6" s="8" t="s">
+      <c r="E6" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1999</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>88</v>
       </c>
       <c r="H6" s="5" t="s">
@@ -918,6 +981,9 @@
       </c>
       <c r="I6" s="5" t="s">
         <v>16</v>
+      </c>
+      <c r="J6" s="5">
+        <v>15585101</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -933,7 +999,12 @@
       <c r="D7" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7" s="5">
+        <v>2006</v>
+      </c>
       <c r="G7" s="5" t="s">
         <v>89</v>
       </c>
@@ -942,6 +1013,9 @@
       </c>
       <c r="I7" s="5" t="s">
         <v>16</v>
+      </c>
+      <c r="J7" s="5">
+        <v>17451347</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -957,12 +1031,23 @@
       <c r="D8" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="E8" s="5"/>
+      <c r="E8" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="5">
+        <v>2005</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>89</v>
+      </c>
       <c r="H8" s="5" t="s">
         <v>68</v>
       </c>
       <c r="I8" s="5" t="s">
         <v>16</v>
+      </c>
+      <c r="J8" s="5">
+        <v>24324545</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -978,12 +1063,23 @@
       <c r="D9" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="E9" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" s="5">
+        <v>2004</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>96</v>
+      </c>
       <c r="H9" s="5" t="s">
         <v>68</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>16</v>
+      </c>
+      <c r="J9" s="5">
+        <v>26699702</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -997,12 +1093,23 @@
         <v>20</v>
       </c>
       <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="E10" t="s">
+        <v>100</v>
+      </c>
+      <c r="F10" s="5">
+        <v>1995</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="H10" s="5" t="s">
         <v>68</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>16</v>
+      </c>
+      <c r="J10" s="5">
+        <v>9734396</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -1016,12 +1123,23 @@
         <v>24</v>
       </c>
       <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="E11" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" s="5">
+        <v>2005</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="H11" s="5" t="s">
         <v>68</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>16</v>
+      </c>
+      <c r="J11" s="5">
+        <v>26699702</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -1035,12 +1153,23 @@
         <v>27</v>
       </c>
       <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="E12" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" s="5">
+        <v>2009</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="H12" s="5" t="s">
         <v>68</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>16</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -1069,7 +1198,9 @@
       <c r="I13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="J13" s="5"/>
+      <c r="J13" s="5">
+        <v>25733890</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
@@ -1097,7 +1228,9 @@
       <c r="I14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="J14" s="5"/>
+      <c r="J14" s="5">
+        <v>25733890</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
@@ -1123,7 +1256,9 @@
       <c r="I15" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="J15" s="5"/>
+      <c r="J15" s="5">
+        <v>22505456</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
@@ -1149,7 +1284,9 @@
       <c r="I16" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="J16" s="5"/>
+      <c r="J16" s="5">
+        <v>22505456</v>
+      </c>
     </row>
     <row r="17" spans="1:10" ht="17" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
@@ -1175,7 +1312,9 @@
       <c r="I17" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="J17" s="5"/>
+      <c r="J17" s="5">
+        <v>17494082</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>

<commit_message>
Fully validated build for Groups N,O,P and M subtypes: A (A1-A5), B, C, F1, CRF01
</commit_message>
<xml_diff>
--- a/tabular/core/hiv-reference-data.xlsx
+++ b/tabular/core/hiv-reference-data.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/general/HIV-GLUE/tabular/core/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FFC595-986F-F848-A21B-5C4D180B8142}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="24030"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="29900" yWindow="4100" windowWidth="20380" windowHeight="18480" xr2:uid="{42735871-A8C7-D842-BA39-4089F1652FC4}"/>
+    <workbookView xWindow="29900" yWindow="4100" windowWidth="20380" windowHeight="18480"/>
   </bookViews>
   <sheets>
     <sheet name="main refs" sheetId="1" r:id="rId1"/>
     <sheet name="excluded" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -32,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="105">
   <si>
     <t>Accession</t>
   </si>
@@ -335,18 +332,31 @@
   </si>
   <si>
     <t>YBF30</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>KU168300</t>
+  </si>
+  <si>
+    <t>LA57LmNe</t>
+  </si>
+  <si>
+    <t>Guinea-Bissau</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -390,6 +400,24 @@
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -446,8 +474,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -468,7 +504,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -527,7 +571,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -579,7 +623,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -773,21 +817,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685A96F8-87E5-2E44-B73D-ACDE15C469C7}">
-  <dimension ref="A1:J17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="A1:J17"/>
+      <selection activeCell="J18" sqref="A1:J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="5" max="5" width="21.33203125" customWidth="1"/>
@@ -796,7 +840,7 @@
     <col min="9" max="9" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -828,7 +872,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -860,7 +904,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" s="6" t="s">
         <v>70</v>
       </c>
@@ -892,7 +936,7 @@
         <v>23170185</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" s="6" t="s">
         <v>71</v>
       </c>
@@ -924,7 +968,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" s="6" t="s">
         <v>72</v>
       </c>
@@ -954,9 +998,9 @@
         <v>26699702</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" s="6" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>11</v>
@@ -965,16 +1009,16 @@
         <v>12</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="F6" s="5">
-        <v>1999</v>
+        <v>2008</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>68</v>
@@ -983,12 +1027,12 @@
         <v>16</v>
       </c>
       <c r="J6" s="5">
-        <v>15585101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+        <v>26699702</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>11</v>
@@ -997,16 +1041,16 @@
         <v>12</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F7" s="5">
-        <v>2006</v>
+        <v>1999</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>68</v>
@@ -1015,12 +1059,12 @@
         <v>16</v>
       </c>
       <c r="J7" s="5">
-        <v>17451347</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+        <v>15585101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>11</v>
@@ -1029,13 +1073,13 @@
         <v>12</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F8" s="5">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>89</v>
@@ -1047,12 +1091,12 @@
         <v>16</v>
       </c>
       <c r="J8" s="5">
-        <v>24324545</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+        <v>17451347</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>11</v>
@@ -1061,16 +1105,16 @@
         <v>12</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F9" s="5">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>68</v>
@@ -1079,28 +1123,30 @@
         <v>16</v>
       </c>
       <c r="J9" s="5">
-        <v>26699702</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+        <v>24324545</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" t="s">
-        <v>100</v>
+        <v>12</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>97</v>
       </c>
       <c r="F10" s="5">
-        <v>1995</v>
+        <v>2004</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>22</v>
+        <v>96</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>68</v>
@@ -1109,25 +1155,25 @@
         <v>16</v>
       </c>
       <c r="J10" s="5">
-        <v>9734396</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+        <v>26699702</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D11" s="5"/>
-      <c r="E11" s="5" t="s">
-        <v>98</v>
+      <c r="E11" t="s">
+        <v>100</v>
       </c>
       <c r="F11" s="5">
-        <v>2005</v>
+        <v>1995</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>22</v>
@@ -1139,28 +1185,28 @@
         <v>16</v>
       </c>
       <c r="J11" s="5">
-        <v>26699702</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+        <v>9734396</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F12" s="5">
-        <v>2009</v>
+        <v>2005</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>68</v>
@@ -1168,56 +1214,56 @@
       <c r="I12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J12" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J12" s="5">
+        <v>26699702</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>30</v>
+        <v>79</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5" t="s">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="F13" s="5">
-        <v>2013</v>
+        <v>2009</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J13" s="5">
-        <v>25733890</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F14" s="5">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>22</v>
@@ -1232,47 +1278,49 @@
         <v>25733890</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F15" s="5"/>
+        <v>66</v>
+      </c>
+      <c r="F15" s="5">
+        <v>2012</v>
+      </c>
       <c r="G15" s="5" t="s">
         <v>22</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="J15" s="5">
-        <v>22505456</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+        <v>25733890</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5" t="s">
@@ -1288,23 +1336,23 @@
         <v>22505456</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="D17" s="5"/>
-      <c r="E17" s="8" t="s">
-        <v>65</v>
+      <c r="E17" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>69</v>
@@ -1313,26 +1361,60 @@
         <v>50</v>
       </c>
       <c r="J17" s="5">
+        <v>22505456</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="17">
+      <c r="A18" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J18" s="5">
         <v>17494082</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C898F709-88FD-7D4F-BCC8-2857C1587A7E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1364,7 +1446,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" s="5" t="s">
         <v>35</v>
       </c>
@@ -1394,7 +1476,7 @@
         <v>25900654</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" s="5" t="s">
         <v>29</v>
       </c>
@@ -1424,7 +1506,7 @@
         <v>19073717</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" s="5" t="s">
         <v>44</v>
       </c>
@@ -1454,7 +1536,7 @@
         <v>2188136</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" s="5" t="s">
         <v>45</v>
       </c>
@@ -1484,7 +1566,7 @@
         <v>9989410</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" s="5" t="s">
         <v>46</v>
       </c>
@@ -1514,7 +1596,7 @@
         <v>21775446</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8" s="6" t="s">
         <v>39</v>
       </c>
@@ -1546,7 +1628,7 @@
         <v>12487816</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" s="6" t="s">
         <v>38</v>
       </c>
@@ -1578,7 +1660,7 @@
         <v>8891112</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10">
       <c r="A10" s="6" t="s">
         <v>19</v>
       </c>
@@ -1608,7 +1690,7 @@
         <v>16438650</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11" s="7" t="s">
         <v>54</v>
       </c>
@@ -1638,7 +1720,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" s="6" t="s">
         <v>23</v>
       </c>
@@ -1668,7 +1750,7 @@
         <v>8107219</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13" s="6" t="s">
         <v>26</v>
       </c>
@@ -1700,5 +1782,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added AB049811 as CRF02 reference sequence - updated tabular data & hiv-refseqs source.
</commit_message>
<xml_diff>
--- a/tabular/core/hiv-reference-data.xlsx
+++ b/tabular/core/hiv-reference-data.xlsx
@@ -1,35 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="24030"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/general/HIV-GLUE/tabular/core/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA271B9-A5A2-DD40-A480-651337F63B55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29900" yWindow="4100" windowWidth="20380" windowHeight="18480"/>
+    <workbookView xWindow="740" yWindow="460" windowWidth="28060" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main refs" sheetId="1" r:id="rId1"/>
     <sheet name="excluded" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="109">
   <si>
     <t>Accession</t>
   </si>
@@ -344,12 +344,24 @@
   </si>
   <si>
     <t>Guinea-Bissau</t>
+  </si>
+  <si>
+    <t>AB049811</t>
+  </si>
+  <si>
+    <t>CRF02</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>Ghana</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -571,7 +583,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -623,7 +635,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -817,21 +829,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="A1:J18"/>
+      <selection activeCell="J19" sqref="A1:J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="5" max="5" width="21.33203125" customWidth="1"/>
@@ -840,7 +852,7 @@
     <col min="9" max="9" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -872,9 +884,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>11</v>
@@ -883,16 +895,16 @@
         <v>12</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>14</v>
+        <v>91</v>
       </c>
       <c r="F2" s="5">
-        <v>1983</v>
+        <v>2012</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>15</v>
+        <v>87</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>68</v>
@@ -904,9 +916,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>11</v>
@@ -915,16 +927,16 @@
         <v>12</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="F3" s="5">
-        <v>1981</v>
+        <v>1983</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>86</v>
+        <v>15</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>68</v>
@@ -932,13 +944,13 @@
       <c r="I3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="5">
-        <v>23170185</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="J3" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>11</v>
@@ -947,16 +959,16 @@
         <v>12</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>80</v>
+        <v>18</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F4" s="5">
-        <v>2012</v>
+        <v>1981</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>68</v>
@@ -964,13 +976,13 @@
       <c r="I4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="J4" s="5">
+        <v>23170185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>11</v>
@@ -979,15 +991,17 @@
         <v>12</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F5" s="5">
-        <v>2003</v>
-      </c>
-      <c r="G5" s="5"/>
+        <v>2006</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>89</v>
+      </c>
       <c r="H5" s="5" t="s">
         <v>68</v>
       </c>
@@ -995,30 +1009,30 @@
         <v>16</v>
       </c>
       <c r="J5" s="5">
-        <v>26699702</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>17451347</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B6" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>103</v>
+        <v>106</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>107</v>
       </c>
       <c r="F6" s="5">
-        <v>2008</v>
+        <v>1993</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>68</v>
@@ -1027,12 +1041,12 @@
         <v>16</v>
       </c>
       <c r="J6" s="5">
-        <v>26699702</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>1375062</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>11</v>
@@ -1041,16 +1055,16 @@
         <v>12</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F7" s="5">
-        <v>1999</v>
+        <v>2005</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>68</v>
@@ -1059,12 +1073,12 @@
         <v>16</v>
       </c>
       <c r="J7" s="5">
-        <v>15585101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>24324545</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>11</v>
@@ -1073,16 +1087,16 @@
         <v>12</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F8" s="5">
-        <v>2006</v>
+        <v>1999</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>68</v>
@@ -1091,12 +1105,12 @@
         <v>16</v>
       </c>
       <c r="J8" s="5">
-        <v>17451347</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>15585101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>11</v>
@@ -1105,17 +1119,15 @@
         <v>12</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F9" s="5">
-        <v>2005</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>89</v>
-      </c>
+        <v>2003</v>
+      </c>
+      <c r="G9" s="5"/>
       <c r="H9" s="5" t="s">
         <v>68</v>
       </c>
@@ -1123,12 +1135,12 @@
         <v>16</v>
       </c>
       <c r="J9" s="5">
-        <v>24324545</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <v>26699702</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>11</v>
@@ -1137,16 +1149,16 @@
         <v>12</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="F10" s="5">
-        <v>2004</v>
+        <v>2008</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>68</v>
@@ -1158,25 +1170,27 @@
         <v>26699702</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" t="s">
-        <v>100</v>
+        <v>12</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>97</v>
       </c>
       <c r="F11" s="5">
-        <v>1995</v>
+        <v>2004</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>22</v>
+        <v>96</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>68</v>
@@ -1185,25 +1199,25 @@
         <v>16</v>
       </c>
       <c r="J11" s="5">
-        <v>9734396</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>26699702</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D12" s="5"/>
-      <c r="E12" s="5" t="s">
-        <v>98</v>
+      <c r="E12" t="s">
+        <v>100</v>
       </c>
       <c r="F12" s="5">
-        <v>2005</v>
+        <v>1995</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>22</v>
@@ -1215,28 +1229,28 @@
         <v>16</v>
       </c>
       <c r="J12" s="5">
-        <v>26699702</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>9734396</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F13" s="5">
-        <v>2009</v>
+        <v>2005</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>68</v>
@@ -1244,71 +1258,69 @@
       <c r="I13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J13" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="J13" s="5">
+        <v>26699702</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>30</v>
+        <v>79</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5" t="s">
-        <v>67</v>
+        <v>99</v>
       </c>
       <c r="F14" s="5">
-        <v>2013</v>
+        <v>2009</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J14" s="5">
-        <v>25733890</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>16</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" s="5">
-        <v>2012</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="F15" s="5"/>
       <c r="G15" s="5" t="s">
         <v>22</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="J15" s="5">
-        <v>25733890</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+        <v>22505456</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>59</v>
       </c>
@@ -1336,23 +1348,23 @@
         <v>22505456</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" ht="17" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="D17" s="5"/>
-      <c r="E17" s="5" t="s">
-        <v>63</v>
+      <c r="E17" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>69</v>
@@ -1361,38 +1373,75 @@
         <v>50</v>
       </c>
       <c r="J17" s="5">
-        <v>22505456</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="17">
+        <v>17494082</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>62</v>
+        <v>24</v>
       </c>
       <c r="D18" s="5"/>
-      <c r="E18" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" s="5"/>
+      <c r="E18" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="5">
+        <v>2012</v>
+      </c>
       <c r="G18" s="5" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="J18" s="5">
-        <v>17494082</v>
+        <v>25733890</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="5">
+        <v>2013</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J19" s="5">
+        <v>25733890</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J19">
+    <sortCondition ref="B2:B19"/>
+    <sortCondition ref="C2:C19"/>
+    <sortCondition ref="D2:D19"/>
+  </sortState>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1405,16 +1454,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1446,7 +1495,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>35</v>
       </c>
@@ -1476,7 +1525,7 @@
         <v>25900654</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>29</v>
       </c>
@@ -1506,7 +1555,7 @@
         <v>19073717</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>44</v>
       </c>
@@ -1536,7 +1585,7 @@
         <v>2188136</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>45</v>
       </c>
@@ -1566,7 +1615,7 @@
         <v>9989410</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>46</v>
       </c>
@@ -1596,7 +1645,7 @@
         <v>21775446</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>39</v>
       </c>
@@ -1628,7 +1677,7 @@
         <v>12487816</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>38</v>
       </c>
@@ -1660,7 +1709,7 @@
         <v>8891112</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>19</v>
       </c>
@@ -1690,7 +1739,7 @@
         <v>16438650</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>54</v>
       </c>
@@ -1720,7 +1769,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>23</v>
       </c>
@@ -1750,7 +1799,7 @@
         <v>8107219</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Incoroprating CRF02 into extension project
</commit_message>
<xml_diff>
--- a/tabular/core/hiv-reference-data.xlsx
+++ b/tabular/core/hiv-reference-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/general/HIV-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA271B9-A5A2-DD40-A480-651337F63B55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1AFFE39-4609-7540-8F76-FAA7AF0F1E0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="460" windowWidth="28060" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -840,7 +840,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="A1:J19"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1029,7 +1029,7 @@
         <v>107</v>
       </c>
       <c r="F6" s="5">
-        <v>1993</v>
+        <v>1997</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>108</v>

</xml_diff>

<commit_message>
Subtypes D and G brought into extension build
</commit_message>
<xml_diff>
--- a/tabular/core/hiv-reference-data.xlsx
+++ b/tabular/core/hiv-reference-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/general/HIV-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1AFFE39-4609-7540-8F76-FAA7AF0F1E0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C02855F-BA05-5E48-8716-0EC72D13A5CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="460" windowWidth="28060" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="113">
   <si>
     <t>Accession</t>
   </si>
@@ -356,6 +356,18 @@
   </si>
   <si>
     <t>Ghana</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>AB485648</t>
+  </si>
+  <si>
+    <t>Senegal</t>
+  </si>
+  <si>
+    <t>SE365</t>
   </si>
 </sst>
 </file>
@@ -837,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="J9" sqref="A1:J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -982,7 +994,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>74</v>
+        <v>110</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>11</v>
@@ -991,16 +1003,16 @@
         <v>12</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>83</v>
+        <v>109</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="F5" s="5">
-        <v>2006</v>
+        <v>1990</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>68</v>
@@ -1008,31 +1020,29 @@
       <c r="I5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="5">
-        <v>17451347</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B6" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>107</v>
+        <v>83</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>94</v>
       </c>
       <c r="F6" s="5">
-        <v>1997</v>
+        <v>2006</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>68</v>
@@ -1041,30 +1051,30 @@
         <v>16</v>
       </c>
       <c r="J6" s="5">
-        <v>1375062</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+        <v>17451347</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>95</v>
+        <v>106</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>107</v>
       </c>
       <c r="F7" s="5">
-        <v>2005</v>
+        <v>1997</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>68</v>
@@ -1073,12 +1083,12 @@
         <v>16</v>
       </c>
       <c r="J7" s="5">
-        <v>24324545</v>
+        <v>1375062</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>11</v>
@@ -1087,16 +1097,16 @@
         <v>12</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F8" s="5">
-        <v>1999</v>
+        <v>2005</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>68</v>
@@ -1105,12 +1115,12 @@
         <v>16</v>
       </c>
       <c r="J8" s="5">
-        <v>15585101</v>
+        <v>24324545</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>11</v>
@@ -1119,15 +1129,17 @@
         <v>12</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F9" s="5">
-        <v>2003</v>
-      </c>
-      <c r="G9" s="5"/>
+        <v>1999</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>88</v>
+      </c>
       <c r="H9" s="5" t="s">
         <v>68</v>
       </c>
@@ -1135,12 +1147,12 @@
         <v>16</v>
       </c>
       <c r="J9" s="5">
-        <v>26699702</v>
+        <v>15585101</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>11</v>
@@ -1149,17 +1161,15 @@
         <v>12</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="F10" s="5">
-        <v>2008</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>104</v>
-      </c>
+        <v>2003</v>
+      </c>
+      <c r="G10" s="5"/>
       <c r="H10" s="5" t="s">
         <v>68</v>
       </c>
@@ -1172,7 +1182,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>11</v>
@@ -1181,16 +1191,16 @@
         <v>12</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="F11" s="5">
-        <v>2004</v>
+        <v>2008</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>68</v>
@@ -1204,23 +1214,25 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" t="s">
-        <v>100</v>
+        <v>12</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>97</v>
       </c>
       <c r="F12" s="5">
-        <v>1995</v>
+        <v>2004</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>22</v>
+        <v>96</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>68</v>
@@ -1229,25 +1241,25 @@
         <v>16</v>
       </c>
       <c r="J12" s="5">
-        <v>9734396</v>
+        <v>26699702</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D13" s="5"/>
-      <c r="E13" s="5" t="s">
-        <v>98</v>
+      <c r="E13" t="s">
+        <v>100</v>
       </c>
       <c r="F13" s="5">
-        <v>2005</v>
+        <v>1995</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>22</v>
@@ -1259,28 +1271,28 @@
         <v>16</v>
       </c>
       <c r="J13" s="5">
-        <v>26699702</v>
+        <v>9734396</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F14" s="5">
-        <v>2009</v>
+        <v>2005</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>68</v>
@@ -1288,51 +1300,53 @@
       <c r="I14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J14" s="5" t="s">
-        <v>52</v>
+      <c r="J14" s="5">
+        <v>26699702</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>36</v>
+        <v>79</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" s="5"/>
+        <v>99</v>
+      </c>
+      <c r="F15" s="5">
+        <v>2009</v>
+      </c>
       <c r="G15" s="5" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="J15" s="5">
-        <v>22505456</v>
+        <v>16</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5" t="s">
@@ -1348,23 +1362,23 @@
         <v>22505456</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="D17" s="5"/>
-      <c r="E17" s="8" t="s">
-        <v>65</v>
+      <c r="E17" s="5" t="s">
+        <v>64</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>69</v>
@@ -1373,55 +1387,53 @@
         <v>50</v>
       </c>
       <c r="J17" s="5">
+        <v>22505456</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="J18" s="5">
         <v>17494082</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18" s="5">
-        <v>2012</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J18" s="5">
-        <v>25733890</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F19" s="5">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>22</v>
@@ -1436,11 +1448,41 @@
         <v>25733890</v>
       </c>
     </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="5">
+        <v>2013</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J20" s="5">
+        <v>25733890</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J19">
-    <sortCondition ref="B2:B19"/>
-    <sortCondition ref="C2:C19"/>
-    <sortCondition ref="D2:D19"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J20">
+    <sortCondition ref="B2:B20"/>
+    <sortCondition ref="C2:C20"/>
+    <sortCondition ref="D2:D20"/>
   </sortState>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>